<commit_message>
asset return data addition
</commit_message>
<xml_diff>
--- a/data/Asset Return Data.xlsx
+++ b/data/Asset Return Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\twang\Documents\asset_simulations\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53C16929-792B-44E1-99D6-7C770A0A4744}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{068268FB-F8CC-4473-89A1-CD2CDF5CBC7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="150" windowWidth="29040" windowHeight="17640" xr2:uid="{21C042B3-50D8-4AF8-A904-9660A755F6A9}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{21C042B3-50D8-4AF8-A904-9660A755F6A9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -470,7 +470,7 @@
   <dimension ref="A1:K567"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="L30" sqref="L30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
starting simulation anlysis nb
</commit_message>
<xml_diff>
--- a/data/Asset Return Data.xlsx
+++ b/data/Asset Return Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\twang\Documents\asset_simulations\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{068268FB-F8CC-4473-89A1-CD2CDF5CBC7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{911913DF-E4A1-4B1B-B004-7EC3DF94FBFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{21C042B3-50D8-4AF8-A904-9660A755F6A9}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{21C042B3-50D8-4AF8-A904-9660A755F6A9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>3-5Y US Treasury</t>
   </si>
@@ -64,6 +64,9 @@
   </si>
   <si>
     <t>US3M T-Bill</t>
+  </si>
+  <si>
+    <t>Date</t>
   </si>
 </sst>
 </file>
@@ -470,7 +473,7 @@
   <dimension ref="A1:K567"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L30" sqref="L30"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -481,6 +484,9 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="B1" s="3" t="s">
         <v>5</v>
       </c>

</xml_diff>